<commit_message>
corrected data for months of Jan, oct, nov. and remade graphs to be more accurate
</commit_message>
<xml_diff>
--- a/Kevin data process/Analysis.xlsx
+++ b/Kevin data process/Analysis.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Graphs" sheetId="1" r:id="rId1"/>
+    <sheet name="2011 Data" sheetId="2" r:id="rId2"/>
+    <sheet name="2014 Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="116">
   <si>
     <t>Months:</t>
   </si>
@@ -276,12 +277,6 @@
     <t>lib/</t>
   </si>
   <si>
-    <t>^ Missing data?</t>
-  </si>
-  <si>
-    <t>Miss Data</t>
-  </si>
-  <si>
     <t>jstests/parallel/</t>
   </si>
   <si>
@@ -376,6 +371,9 @@
   </si>
   <si>
     <t>Issues</t>
+  </si>
+  <si>
+    <t>Months</t>
   </si>
 </sst>
 </file>
@@ -426,7 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -434,6 +432,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,7 +538,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$7</c:f>
+              <c:f>Graphs!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -550,7 +549,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -559,52 +558,17 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$6:$M$6</c:f>
-              <c:strCache>
+            <c:numRef>
+              <c:f>Graphs!$B$6:$M$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>Janurary</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>February</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>March</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>April</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>May</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>June</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>July</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>August</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>September</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>October</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>November</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>December</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$M$7</c:f>
+              <c:f>Graphs!$B$4:$M$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -658,11 +622,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="713290640"/>
-        <c:axId val="713285936"/>
+        <c:axId val="627577736"/>
+        <c:axId val="627578128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="713290640"/>
+        <c:axId val="627577736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -761,7 +725,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="713285936"/>
+        <c:crossAx val="627578128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -769,7 +733,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="713285936"/>
+        <c:axId val="627578128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,7 +840,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="713290640"/>
+        <c:crossAx val="627577736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1007,7 +971,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>Graphs!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1028,7 +992,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$M$2</c:f>
+              <c:f>Graphs!$B$2:$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1072,12 +1036,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$M$3</c:f>
+              <c:f>Graphs!$B$3:$M$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>49.544697292971854</c:v>
+                  <c:v>49.646959715186867</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>70.445705838563896</c:v>
@@ -1104,10 +1068,10 @@
                   <c:v>65.841093060572135</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>59.496626987580697</c:v>
+                  <c:v>71.950218337776391</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>62.382667441780463</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>49.148754824102483</c:v>
@@ -1126,11 +1090,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="739593536"/>
-        <c:axId val="739593144"/>
+        <c:axId val="627578520"/>
+        <c:axId val="612331896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="739593536"/>
+        <c:axId val="627578520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1229,7 +1193,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="739593144"/>
+        <c:crossAx val="612331896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1237,7 +1201,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="739593144"/>
+        <c:axId val="612331896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,7 +1308,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="739593536"/>
+        <c:crossAx val="627578520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1428,13 +1392,12 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
-              <a:t>Number</a:t>
+              <a:t>Ownership</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-CA" baseline="0"/>
-              <a:t> of Issue vs Ownership</a:t>
+              <a:t> vs Number of Issues</a:t>
             </a:r>
-            <a:endParaRPr lang="en-CA"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1479,11 +1442,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$7</c:f>
+              <c:f>Graphs!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Issues</c:v>
+                  <c:v>Adjusted Ownership Lv</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1514,7 +1477,7 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$B$6:$M$6</c:f>
+              <c:f>Graphs!$B$2:$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1558,7 +1521,136 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$M$7</c:f>
+              <c:f>Graphs!$B$3:$M$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>49.646959715186867</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.445705838563896</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.656074018251672</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.606786073483235</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59.811202562470072</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44.245469492142419</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70.395834966871831</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>98.281575126903107</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>65.841093060572135</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>71.950218337776391</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>62.382667441780463</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>49.148754824102483</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graphs!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Issues</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Graphs!$B$2:$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Janurary</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>November</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>December</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Graphs!$B$4:$M$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1603,135 +1695,6 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Adjusted Ownership Lv</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$B$6:$M$6</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>Janurary</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>February</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>March</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>April</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>May</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>June</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>July</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>August</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>September</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>October</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>November</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>December</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$8:$M$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>49.544697292971854</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>70.445705838563896</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>77.656074018251672</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>56.606786073483235</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>59.811202562470072</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>44.245469492142419</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70.395834966871831</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>98.281575126903107</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>65.841093060572135</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>59.496626987580697</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>49.148754824102483</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1740,11 +1703,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="531035352"/>
-        <c:axId val="531036136"/>
+        <c:axId val="612330328"/>
+        <c:axId val="612330720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="531035352"/>
+        <c:axId val="612330328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1800,12 +1763,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="531036136"/>
+        <c:crossAx val="612330720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="531036136"/>
+        <c:axId val="612330720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1862,7 +1825,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="531035352"/>
+        <c:crossAx val="612330328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1944,12 +1907,9 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -3591,13 +3551,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3620,14 +3580,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3649,20 +3609,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>147637</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>452437</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3943,10 +3903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V27" sqref="V27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3955,14 +3915,18 @@
     <col min="10" max="10" width="10.85546875" customWidth="1"/>
     <col min="12" max="12" width="10.42578125" customWidth="1"/>
     <col min="13" max="13" width="9.85546875" customWidth="1"/>
+    <col min="15" max="15" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2011</v>
       </c>
+      <c r="O1">
+        <v>2014</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4002,13 +3966,52 @@
       <c r="M2" t="s">
         <v>13</v>
       </c>
+      <c r="O2" t="s">
+        <v>115</v>
+      </c>
+      <c r="P2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>49.544697292971854</v>
+      <c r="B3" s="2">
+        <v>49.646959715186867</v>
       </c>
       <c r="C3" s="1">
         <v>70.445705838563896</v>
@@ -4034,146 +4037,67 @@
       <c r="J3">
         <v>65.841093060572135</v>
       </c>
-      <c r="K3" s="3">
-        <v>59.496626987580697</v>
+      <c r="K3">
+        <v>71.950218337776391</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>62.382667441780463</v>
       </c>
       <c r="M3">
         <v>49.148754824102483</v>
       </c>
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K4" t="s">
-        <v>83</v>
-      </c>
-      <c r="L4" t="s">
-        <v>84</v>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>36</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>57</v>
+      </c>
+      <c r="H4">
+        <v>17</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <v>42</v>
+      </c>
+      <c r="L4">
+        <v>13</v>
+      </c>
+      <c r="M4">
+        <v>8</v>
+      </c>
+      <c r="O4" t="s">
+        <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" t="s">
-        <v>12</v>
-      </c>
-      <c r="M6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B7">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>36</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>57</v>
-      </c>
-      <c r="H7">
-        <v>17</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-      <c r="J7">
-        <v>16</v>
-      </c>
-      <c r="K7">
-        <v>42</v>
-      </c>
-      <c r="L7">
-        <v>13</v>
-      </c>
-      <c r="M7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>49.544697292971854</v>
-      </c>
-      <c r="C8" s="1">
-        <v>70.445705838563896</v>
-      </c>
-      <c r="D8">
-        <v>77.656074018251672</v>
-      </c>
-      <c r="E8" s="2">
-        <v>56.606786073483235</v>
-      </c>
-      <c r="F8">
-        <v>59.811202562470072</v>
-      </c>
-      <c r="G8">
-        <v>44.245469492142419</v>
-      </c>
-      <c r="H8">
-        <v>70.395834966871831</v>
-      </c>
-      <c r="I8">
-        <v>98.281575126903107</v>
-      </c>
-      <c r="J8">
-        <v>65.841093060572135</v>
-      </c>
-      <c r="K8" s="3">
-        <v>59.496626987580697</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>49.148754824102483</v>
-      </c>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="K8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4185,8 +4109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BB7" sqref="BB7"/>
+    <sheetView topLeftCell="AN1" workbookViewId="0">
+      <selection sqref="A1:BG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4380,13 +4304,15 @@
         <v>19</v>
       </c>
       <c r="B3">
-        <v>2.8676646875813391E-2</v>
-      </c>
-      <c r="C3">
+        <f ca="1">(#REF!/B$35)*100</f>
+        <v>2.8637213569337003E-2</v>
+      </c>
+      <c r="C3" s="5">
         <v>0.65</v>
       </c>
-      <c r="D3">
-        <v>1.8639820469278704E-2</v>
+      <c r="D3" s="2">
+        <f ca="1">B3*C3</f>
+        <v>1.8614188820069051E-2</v>
       </c>
       <c r="F3" t="s">
         <v>48</v>
@@ -4490,7 +4416,7 @@
       <c r="AU3">
         <v>0.15311376724082329</v>
       </c>
-      <c r="AV3" s="4">
+      <c r="AV3" s="7">
         <v>0.76827357360125359</v>
       </c>
       <c r="AW3">
@@ -4501,6 +4427,12 @@
       </c>
       <c r="AZ3">
         <v>3.8346658614598766E-2</v>
+      </c>
+      <c r="BA3" s="7">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="BB3">
+        <v>2.7390470438999118E-2</v>
       </c>
       <c r="BD3" t="s">
         <v>22</v>
@@ -4520,13 +4452,15 @@
         <v>20</v>
       </c>
       <c r="B4">
-        <v>1.4338323437906694E-3</v>
-      </c>
-      <c r="C4">
-        <v>92.02000000000001</v>
-      </c>
-      <c r="D4">
-        <v>0.13194125227561743</v>
+        <f t="shared" ref="B4" ca="1" si="0">(#REF!/B$35)*100</f>
+        <v>0.13942027426231718</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.94505494505494514</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D35" ca="1" si="1">B4*C4</f>
+        <v>0.13175981963251954</v>
       </c>
       <c r="F4" t="s">
         <v>55</v>
@@ -4630,7 +4564,7 @@
       <c r="AU4">
         <v>9.2935215898315174E-2</v>
       </c>
-      <c r="AV4" s="4">
+      <c r="AV4" s="7">
         <v>0.5315110098709187</v>
       </c>
       <c r="AW4">
@@ -4642,8 +4576,14 @@
       <c r="AZ4">
         <v>4.3824752702398592E-2</v>
       </c>
+      <c r="BA4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="BB4">
+        <v>2.1912376351199296E-2</v>
+      </c>
       <c r="BD4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="BE4">
         <v>2.0319909451120984E-3</v>
@@ -4660,13 +4600,15 @@
         <v>21</v>
       </c>
       <c r="B5">
-        <v>1.8496437234899635E-2</v>
-      </c>
-      <c r="C5">
+        <f t="shared" ref="B5" ca="1" si="2">(#REF!/B$35)*100</f>
+        <v>1.8471002752222365E-2</v>
+      </c>
+      <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5">
-        <v>1.8496437234899635E-2</v>
+      <c r="D5" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.8471002752222365E-2</v>
       </c>
       <c r="F5" t="s">
         <v>56</v>
@@ -4770,17 +4712,23 @@
       <c r="AU5">
         <v>1.7651340094764281</v>
       </c>
-      <c r="AV5" s="4">
-        <v>0.42104021747821224</v>
+      <c r="AV5" s="7">
+        <v>0.58261373630766777</v>
       </c>
       <c r="AW5">
-        <v>0.74319240722814406</v>
+        <v>1.0283913203447961</v>
       </c>
       <c r="AY5" t="s">
         <v>43</v>
       </c>
       <c r="AZ5">
         <v>1.1265262244033314</v>
+      </c>
+      <c r="BA5" s="7">
+        <v>0.57867556238511586</v>
+      </c>
+      <c r="BB5">
+        <v>0.651893196448179</v>
       </c>
       <c r="BD5" t="s">
         <v>37</v>
@@ -4800,13 +4748,15 @@
         <v>22</v>
       </c>
       <c r="B6">
-        <v>2.1702486355615572E-2</v>
-      </c>
-      <c r="C6">
+        <f t="shared" ref="B6" ca="1" si="3">(#REF!/B$35)*100</f>
+        <v>2.167264322927424E-2</v>
+      </c>
+      <c r="C6" s="5">
         <v>0.88636363636363635</v>
       </c>
-      <c r="D6">
-        <v>1.9236294724295621E-2</v>
+      <c r="D6" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.9209842862311258E-2</v>
       </c>
       <c r="F6" t="s">
         <v>50</v>
@@ -4910,17 +4860,23 @@
       <c r="AU6">
         <v>2.7484690387422006</v>
       </c>
-      <c r="AV6" s="4">
-        <v>0.58156820457521374</v>
+      <c r="AV6" s="7">
+        <v>1</v>
       </c>
       <c r="AW6">
-        <v>1.5984222041918652</v>
+        <v>2.7484690387422006</v>
       </c>
       <c r="AY6" t="s">
         <v>40</v>
       </c>
       <c r="AZ6">
         <v>1.2486219854322138</v>
+      </c>
+      <c r="BA6" s="7">
+        <v>0.33316807791865921</v>
+      </c>
+      <c r="BB6">
+        <v>0.41600098693343079</v>
       </c>
       <c r="BD6" t="s">
         <v>32</v>
@@ -4940,13 +4896,15 @@
         <v>23</v>
       </c>
       <c r="B7">
-        <v>7.9835784902264478E-3</v>
-      </c>
-      <c r="C7">
+        <f t="shared" ref="B7" ca="1" si="4">(#REF!/B$35)*100</f>
+        <v>7.9726002577034227E-3</v>
+      </c>
+      <c r="C7" s="5">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D7">
-        <v>4.6570874526320949E-3</v>
+      <c r="D7" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.6506834836603306E-3</v>
       </c>
       <c r="F7" t="s">
         <v>46</v>
@@ -5050,17 +5008,23 @@
       <c r="AU7">
         <v>20.234092306615363</v>
       </c>
-      <c r="AV7" s="4">
-        <v>0.39780798394088596</v>
+      <c r="AV7" s="7">
+        <v>0.76867803164253701</v>
       </c>
       <c r="AW7">
-        <v>8.0492834673684488</v>
+        <v>15.553502246322498</v>
       </c>
       <c r="AY7" t="s">
         <v>25</v>
       </c>
       <c r="AZ7">
         <v>4.1823824055888821</v>
+      </c>
+      <c r="BA7" s="7">
+        <v>0.36810683795387922</v>
+      </c>
+      <c r="BB7">
+        <v>1.5395635624352622</v>
       </c>
       <c r="BD7" t="s">
         <v>70</v>
@@ -5080,13 +5044,15 @@
         <v>24</v>
       </c>
       <c r="B8">
-        <v>1.7865551003631742E-3</v>
-      </c>
-      <c r="C8">
+        <f t="shared" ref="B8" ca="1" si="5">(#REF!/B$35)*100</f>
+        <v>1.7840984053696953E-3</v>
+      </c>
+      <c r="C8" s="5">
         <v>0.9935794542536116</v>
       </c>
-      <c r="D8">
-        <v>1.7750844416128488E-3</v>
+      <c r="D8" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.7726435199419605E-3</v>
       </c>
       <c r="F8" t="s">
         <v>33</v>
@@ -5190,17 +5156,23 @@
       <c r="AU8">
         <v>2.8011393843355967</v>
       </c>
-      <c r="AV8" s="4">
-        <v>0.98358248058969033</v>
+      <c r="AV8" s="7">
+        <v>0.59626052388941775</v>
       </c>
       <c r="AW8">
-        <v>2.7551516241222842</v>
+        <v>1.670208836791224</v>
       </c>
       <c r="AY8" t="s">
         <v>49</v>
       </c>
       <c r="AZ8">
         <v>21.026557581013886</v>
+      </c>
+      <c r="BA8" s="7">
+        <v>0.56736579598561665</v>
+      </c>
+      <c r="BB8">
+        <v>11.929749578789346</v>
       </c>
       <c r="BD8" t="s">
         <v>41</v>
@@ -5220,13 +5192,15 @@
         <v>25</v>
       </c>
       <c r="B9">
-        <v>2.6798326505447609E-3</v>
-      </c>
-      <c r="C9">
+        <f t="shared" ref="B9" ca="1" si="6">(#REF!/B$35)*100</f>
+        <v>2.6761476080545427E-3</v>
+      </c>
+      <c r="C9" s="5">
         <v>0.9935794542536116</v>
       </c>
-      <c r="D9">
-        <v>2.662626662419273E-3</v>
+      <c r="D9" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.6589652799129406E-3</v>
       </c>
       <c r="F9" t="s">
         <v>41</v>
@@ -5330,7 +5304,7 @@
       <c r="AU9">
         <v>3.9730898567104092</v>
       </c>
-      <c r="AV9" s="4">
+      <c r="AV9" s="7">
         <v>0.9996057069479054</v>
       </c>
       <c r="AW9">
@@ -5341,6 +5315,12 @@
       </c>
       <c r="AZ9">
         <v>1.4585973318175811</v>
+      </c>
+      <c r="BA9" s="7">
+        <v>0.96619845264027637</v>
+      </c>
+      <c r="BB9">
+        <v>1.4092944850273825</v>
       </c>
       <c r="BD9" t="s">
         <v>27</v>
@@ -5360,13 +5340,15 @@
         <v>26</v>
       </c>
       <c r="B10">
-        <v>1.4338323437906694E-3</v>
-      </c>
-      <c r="C10">
-        <v>0.59</v>
-      </c>
-      <c r="D10">
-        <v>8.4596108283649493E-4</v>
+        <f t="shared" ref="B10" ca="1" si="7">(#REF!/B$35)*100</f>
+        <v>9.5361921185892207E-4</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.8858858858858859</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.4479780029544146E-4</v>
       </c>
       <c r="F10" t="s">
         <v>23</v>
@@ -5470,11 +5452,11 @@
       <c r="AU10">
         <v>0.13546524977979929</v>
       </c>
-      <c r="AV10" s="4">
-        <v>0.50382872323800587</v>
+      <c r="AV10" s="7">
+        <v>0.65880085430015101</v>
       </c>
       <c r="AW10">
-        <v>6.8251283839673826E-2</v>
+        <v>8.9244622282915118E-2</v>
       </c>
       <c r="AY10" t="s">
         <v>32</v>
@@ -5482,8 +5464,14 @@
       <c r="AZ10">
         <v>2.7390470438999122E-2</v>
       </c>
+      <c r="BA10" s="7">
+        <v>1</v>
+      </c>
+      <c r="BB10">
+        <v>2.7390470438999122E-2</v>
+      </c>
       <c r="BD10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="BE10">
         <v>0.50984674658346463</v>
@@ -5500,13 +5488,15 @@
         <v>27</v>
       </c>
       <c r="B11">
-        <v>3.0358532215079843E-2</v>
-      </c>
-      <c r="C11">
+        <f t="shared" ref="B11" ca="1" si="8">(#REF!/B$35)*100</f>
+        <v>3.0316786145178611E-2</v>
+      </c>
+      <c r="C11" s="5">
         <v>0.9379870589902235</v>
       </c>
-      <c r="D11">
-        <v>2.8475910347682699E-2</v>
+      <c r="D11" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.8436753074351642E-2</v>
       </c>
       <c r="F11" t="s">
         <v>30</v>
@@ -5610,11 +5600,11 @@
       <c r="AU11">
         <v>5.3536682454127602</v>
       </c>
-      <c r="AV11" s="4">
-        <v>0.24298219136734081</v>
+      <c r="AV11" s="7">
+        <v>0.54671487339144331</v>
       </c>
       <c r="AW11">
-        <v>1.300846042124139</v>
+        <v>2.9269300569706278</v>
       </c>
       <c r="AY11" t="s">
         <v>70</v>
@@ -5622,8 +5612,14 @@
       <c r="AZ11">
         <v>0.17477311377716556</v>
       </c>
+      <c r="BA11" s="7">
+        <v>0.60083375125376126</v>
+      </c>
+      <c r="BB11">
+        <v>0.10500958556903481</v>
+      </c>
       <c r="BD11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="BE11">
         <v>0.50678317963608177</v>
@@ -5640,13 +5636,15 @@
         <v>28</v>
       </c>
       <c r="B12">
-        <v>1.6718485128599205</v>
-      </c>
-      <c r="C12">
+        <f t="shared" ref="B12" ca="1" si="9">(#REF!/B$35)*100</f>
+        <v>1.669549551092347</v>
+      </c>
+      <c r="C12" s="5">
         <v>0.77778387650085756</v>
       </c>
-      <c r="D12">
-        <v>1.3003368172543828</v>
+      <c r="D12" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.2985487218588723</v>
       </c>
       <c r="F12" t="s">
         <v>34</v>
@@ -5750,7 +5748,7 @@
       <c r="AU12">
         <v>1.4113168701338675E-2</v>
       </c>
-      <c r="AV12" s="4">
+      <c r="AV12" s="7">
         <v>1</v>
       </c>
       <c r="AW12">
@@ -5762,8 +5760,14 @@
       <c r="AZ12">
         <v>0.6134808007045266</v>
       </c>
+      <c r="BA12" s="7">
+        <v>0.94849448155159477</v>
+      </c>
+      <c r="BB12">
+        <v>0.58188315400609714</v>
+      </c>
       <c r="BD12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="BE12">
         <v>1.0141750869447363</v>
@@ -5780,13 +5784,15 @@
         <v>29</v>
       </c>
       <c r="B13">
-        <v>2.7529581000780849E-4</v>
-      </c>
-      <c r="C13">
+        <f t="shared" ref="B13" ca="1" si="10">(#REF!/B$35)*100</f>
+        <v>2.7491725026563521E-4</v>
+      </c>
+      <c r="C13" s="5">
         <v>0.5625</v>
       </c>
-      <c r="D13">
-        <v>1.5485389312939226E-4</v>
+      <c r="D13" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.5464095327441979E-4</v>
       </c>
       <c r="F13" t="s">
         <v>57</v>
@@ -5890,11 +5896,11 @@
       <c r="AU13">
         <v>2.1804845643568256</v>
       </c>
-      <c r="AV13" s="4">
-        <v>0.56005825242718443</v>
+      <c r="AV13" s="7">
+        <v>0.76216181229773461</v>
       </c>
       <c r="AW13">
-        <v>1.2211983745581343</v>
+        <v>1.6618820672574346</v>
       </c>
       <c r="AY13" t="s">
         <v>47</v>
@@ -5902,8 +5908,14 @@
       <c r="AZ13">
         <v>4.1156811319758315</v>
       </c>
+      <c r="BA13" s="7">
+        <v>0.74500531080876042</v>
+      </c>
+      <c r="BB13">
+        <v>3.0662043009174051</v>
+      </c>
       <c r="BD13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="BE13">
         <v>0.10135663592721637</v>
@@ -5920,13 +5932,15 @@
         <v>30</v>
       </c>
       <c r="B14">
-        <v>6.1786330562218144</v>
-      </c>
-      <c r="C14">
+        <f t="shared" ref="B14" ca="1" si="11">(#REF!/B$35)*100</f>
+        <v>6.1701368072717102</v>
+      </c>
+      <c r="C14" s="5">
         <v>0.72727557531907505</v>
       </c>
-      <c r="D14">
-        <v>4.4935689106491754</v>
+      <c r="D14" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.4873897963059344</v>
       </c>
       <c r="F14" t="s">
         <v>32</v>
@@ -6030,7 +6044,7 @@
       <c r="AU14">
         <v>2.1169753052008015E-2</v>
       </c>
-      <c r="AV14" s="4">
+      <c r="AV14" s="7">
         <v>1</v>
       </c>
       <c r="AW14">
@@ -6042,8 +6056,14 @@
       <c r="AZ14">
         <v>1.864178983796017</v>
       </c>
+      <c r="BA14" s="7">
+        <v>0.25135102572164902</v>
+      </c>
+      <c r="BB14">
+        <v>0.46856329970587018</v>
+      </c>
       <c r="BD14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="BE14">
         <v>0.10135663592721637</v>
@@ -6060,13 +6080,15 @@
         <v>31</v>
       </c>
       <c r="B15">
-        <v>0.44021520619061133</v>
-      </c>
-      <c r="C15">
-        <v>5.86281024037522E-2</v>
-      </c>
-      <c r="D15">
-        <v>2.5808982188232049E-2</v>
+        <f t="shared" ref="B15" ca="1" si="12">(#REF!/B$35)*100</f>
+        <v>0.43960986550289227</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.87616441925607458</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.38517052250758266</v>
       </c>
       <c r="F15" t="s">
         <v>37</v>
@@ -6170,7 +6192,7 @@
       <c r="AU15">
         <v>0.16230144006539479</v>
       </c>
-      <c r="AV15" s="4">
+      <c r="AV15" s="7">
         <v>1</v>
       </c>
       <c r="AW15">
@@ -6182,8 +6204,14 @@
       <c r="AZ15">
         <v>0.1369523521949956</v>
       </c>
+      <c r="BA15" s="7">
+        <v>1</v>
+      </c>
+      <c r="BB15">
+        <v>0.1369523521949956</v>
+      </c>
       <c r="BD15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="BE15">
         <v>1.3198686308578134</v>
@@ -6200,13 +6228,15 @@
         <v>32</v>
       </c>
       <c r="B16">
-        <v>0.19614539696587602</v>
-      </c>
-      <c r="C16">
+        <f t="shared" ref="B16" ca="1" si="13">(#REF!/B$35)*100</f>
+        <v>0.19587567709290818</v>
+      </c>
+      <c r="C16" s="5">
         <v>0.97954648459772797</v>
       </c>
-      <c r="D16">
-        <v>0.19213353406794972</v>
+      <c r="D16" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.19186933091455791</v>
       </c>
       <c r="F16" t="s">
         <v>38</v>
@@ -6310,11 +6340,11 @@
       <c r="AU16">
         <v>3.193083248924824</v>
       </c>
-      <c r="AV16" s="4">
-        <v>0.77803167755808311</v>
+      <c r="AV16" s="7">
+        <v>0.64603522233296573</v>
       </c>
       <c r="AW16">
-        <v>2.484319916743595</v>
+        <v>2.0628442466468173</v>
       </c>
       <c r="AY16" t="s">
         <v>39</v>
@@ -6322,8 +6352,14 @@
       <c r="AZ16">
         <v>1.1175311939111641E-2</v>
       </c>
+      <c r="BA16" s="7">
+        <v>1</v>
+      </c>
+      <c r="BB16">
+        <v>1.1175311939111641E-2</v>
+      </c>
       <c r="BD16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="BE16">
         <v>0.40546458918840128</v>
@@ -6340,13 +6376,15 @@
         <v>33</v>
       </c>
       <c r="B17">
-        <v>8.3162275939858823E-2</v>
-      </c>
-      <c r="C17">
+        <f t="shared" ref="B17" ca="1" si="14">(#REF!/B$35)*100</f>
+        <v>8.3047919351077304E-2</v>
+      </c>
+      <c r="C17" s="5">
         <v>0.74137931034482762</v>
       </c>
-      <c r="D17">
-        <v>6.1654790782998785E-2</v>
+      <c r="D17" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>6.1570009174074555E-2</v>
       </c>
       <c r="F17" t="s">
         <v>35</v>
@@ -6450,7 +6488,7 @@
       <c r="AU17">
         <v>2.822633740267735E-2</v>
       </c>
-      <c r="AV17" s="4">
+      <c r="AV17" s="7">
         <v>1</v>
       </c>
       <c r="AW17">
@@ -6462,8 +6500,14 @@
       <c r="AZ17">
         <v>2.2547835265384078E-2</v>
       </c>
+      <c r="BA17" s="7">
+        <v>1</v>
+      </c>
+      <c r="BB17">
+        <v>2.2547835265384078E-2</v>
+      </c>
       <c r="BD17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="BE17">
         <v>0.30406990778164911</v>
@@ -6480,13 +6524,15 @@
         <v>34</v>
       </c>
       <c r="B18">
-        <v>2.6404108640845805</v>
-      </c>
-      <c r="C18">
+        <f t="shared" ref="B18" ca="1" si="15">(#REF!/B$35)*100</f>
+        <v>2.6367800305607756</v>
+      </c>
+      <c r="C18" s="5">
         <v>0.52471564035088669</v>
       </c>
-      <c r="D18">
-        <v>1.3854648773375786</v>
+      <c r="D18" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.3835597222001279</v>
       </c>
       <c r="F18" t="s">
         <v>25</v>
@@ -6590,11 +6636,11 @@
       <c r="AU18">
         <v>0.28226337402677354</v>
       </c>
-      <c r="AV18" s="4">
-        <v>3</v>
+      <c r="AV18" s="7">
+        <v>0.3</v>
       </c>
       <c r="AW18">
-        <v>0.84679012208032067</v>
+        <v>8.4679012208032062E-2</v>
       </c>
       <c r="AY18" t="s">
         <v>57</v>
@@ -6602,8 +6648,14 @@
       <c r="AZ18">
         <v>0.21912376351199297</v>
       </c>
+      <c r="BA18" s="7">
+        <v>1</v>
+      </c>
+      <c r="BB18">
+        <v>0.21912376351199297</v>
+      </c>
       <c r="BD18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="BE18">
         <v>2.0271327185443271</v>
@@ -6620,13 +6672,15 @@
         <v>35</v>
       </c>
       <c r="B19">
-        <v>1.7851685844867287</v>
-      </c>
-      <c r="C19">
+        <f t="shared" ref="B19" ca="1" si="16">(#REF!/B$35)*100</f>
+        <v>1.7827137960936177</v>
+      </c>
+      <c r="C19" s="5">
         <v>0.73452671535613911</v>
       </c>
-      <c r="D19">
-        <v>1.3112540167200051</v>
+      <c r="D19" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.3094509090647188</v>
       </c>
       <c r="F19" t="s">
         <v>47</v>
@@ -6730,11 +6784,11 @@
       <c r="AU19">
         <v>1.7655080084470136</v>
       </c>
-      <c r="AV19" s="4">
-        <v>0.4</v>
+      <c r="AV19" s="7">
+        <v>0.88443321755604676</v>
       </c>
       <c r="AW19">
-        <v>0.70620320337880549</v>
+        <v>1.5614739285317605</v>
       </c>
       <c r="AY19" t="s">
         <v>38</v>
@@ -6742,8 +6796,14 @@
       <c r="AZ19">
         <v>0.42006025465249053</v>
       </c>
+      <c r="BA19" s="7">
+        <v>0.66510172143974955</v>
+      </c>
+      <c r="BB19">
+        <v>0.27938279847779102</v>
+      </c>
       <c r="BD19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="BE19">
         <v>16.014348476500185</v>
@@ -6760,13 +6820,15 @@
         <v>36</v>
       </c>
       <c r="B20">
-        <v>1.4623383646175718</v>
-      </c>
-      <c r="C20">
+        <f t="shared" ref="B20" ca="1" si="17">(#REF!/B$35)*100</f>
+        <v>1.4603275006154495</v>
+      </c>
+      <c r="C20" s="5">
         <v>0.4912337811960415</v>
       </c>
-      <c r="D20">
-        <v>0.71835000423912543</v>
+      <c r="D20" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.71736219991189187</v>
       </c>
       <c r="F20" t="s">
         <v>58</v>
@@ -6870,11 +6932,11 @@
       <c r="AU20">
         <v>2.6360153105299342</v>
       </c>
-      <c r="AV20" s="4">
-        <v>7.5597638622983063E-2</v>
+      <c r="AV20" s="7">
+        <v>0.39489605251181892</v>
       </c>
       <c r="AW20">
-        <v>0.19927653285009245</v>
+        <v>1.0409520404889876</v>
       </c>
       <c r="AY20" t="s">
         <v>35</v>
@@ -6882,8 +6944,14 @@
       <c r="AZ20">
         <v>1.9700431520427484</v>
       </c>
+      <c r="BA20" s="7">
+        <v>0.36149067632124843</v>
+      </c>
+      <c r="BB20">
+        <v>0.71215223141397721</v>
+      </c>
       <c r="BD20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="BE20">
         <v>0.40542654370886549</v>
@@ -6900,13 +6968,15 @@
         <v>37</v>
       </c>
       <c r="B21">
-        <v>4.5762035362865188</v>
-      </c>
-      <c r="C21">
+        <f t="shared" ref="B21" ca="1" si="18">(#REF!/B$35)*100</f>
+        <v>4.5699107909273353</v>
+      </c>
+      <c r="C21" s="5">
         <v>0.76631483565083092</v>
       </c>
-      <c r="D21">
-        <v>3.506812660814155</v>
+      <c r="D21" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.5019904366884398</v>
       </c>
       <c r="F21" t="s">
         <v>51</v>
@@ -7010,11 +7080,11 @@
       <c r="AU21">
         <v>0.45418293856213066</v>
       </c>
-      <c r="AV21" s="4">
-        <v>0.39391895147689487</v>
+      <c r="AV21" s="7">
+        <v>0.35734816587169649</v>
       </c>
       <c r="AW21">
-        <v>0.17891126693708947</v>
+        <v>0.16230144006539479</v>
       </c>
       <c r="AY21" t="s">
         <v>34</v>
@@ -7022,8 +7092,14 @@
       <c r="AZ21">
         <v>2.2806839553855247</v>
       </c>
+      <c r="BA21" s="7">
+        <v>0.37230260755942435</v>
+      </c>
+      <c r="BB21">
+        <v>0.84910458360897267</v>
+      </c>
       <c r="BD21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="BE21">
         <v>4.4596919807975191</v>
@@ -7040,13 +7116,15 @@
         <v>38</v>
       </c>
       <c r="B22">
-        <v>0.12751071033330424</v>
-      </c>
-      <c r="C22">
-        <v>2.4513662431125605</v>
-      </c>
-      <c r="D22">
-        <v>0.31257545094636596</v>
+        <f t="shared" ref="B22" ca="1" si="19">(#REF!/B$35)*100</f>
+        <v>0.127335370136057</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0.96705273810862469</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.12314001834814912</v>
       </c>
       <c r="F22" t="s">
         <v>36</v>
@@ -7150,11 +7228,11 @@
       <c r="AU22">
         <v>0.39767381108197053</v>
       </c>
-      <c r="AV22" s="4">
-        <v>0.71469633174339298</v>
+      <c r="AV22" s="7">
+        <v>1</v>
       </c>
       <c r="AW22">
-        <v>0.2842160140106994</v>
+        <v>0.39767381108197053</v>
       </c>
       <c r="AY22" t="s">
         <v>33</v>
@@ -7162,8 +7240,14 @@
       <c r="AZ22">
         <v>0.24103613986319222</v>
       </c>
+      <c r="BA22" s="7">
+        <v>1</v>
+      </c>
+      <c r="BB22">
+        <v>0.24103613986319222</v>
+      </c>
       <c r="BD22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="BE22">
         <v>0.30406990778164911</v>
@@ -7180,13 +7264,15 @@
         <v>39</v>
       </c>
       <c r="B23">
-        <v>0.9616139996866504</v>
-      </c>
-      <c r="C23">
+        <f t="shared" ref="B23" ca="1" si="20">(#REF!/B$35)*100</f>
+        <v>0.96029168262057774</v>
+      </c>
+      <c r="C23" s="5">
         <v>0.70029523156293794</v>
       </c>
-      <c r="D23">
-        <v>0.67341369858472577</v>
+      <c r="D23" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.67248768624874078</v>
       </c>
       <c r="F23" t="s">
         <v>44</v>
@@ -7290,7 +7376,7 @@
       <c r="AU23">
         <v>2.822633740267735E-2</v>
       </c>
-      <c r="AV23" s="4">
+      <c r="AV23" s="7">
         <v>1</v>
       </c>
       <c r="AW23">
@@ -7300,6 +7386,12 @@
         <v>48</v>
       </c>
       <c r="AZ23">
+        <v>9.8605693580396836E-2</v>
+      </c>
+      <c r="BA23" s="7">
+        <v>1</v>
+      </c>
+      <c r="BB23">
         <v>9.8605693580396836E-2</v>
       </c>
       <c r="BD23" t="s">
@@ -7320,13 +7412,15 @@
         <v>40</v>
       </c>
       <c r="B24">
-        <v>1.811556834941852</v>
-      </c>
-      <c r="C24">
+        <f t="shared" ref="B24" ca="1" si="21">(#REF!/B$35)*100</f>
+        <v>1.8090657600201214</v>
+      </c>
+      <c r="C24" s="5">
         <v>0.68664682132943711</v>
       </c>
-      <c r="D24">
-        <v>1.2438997423704385</v>
+      <c r="D24" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.2421892536937387</v>
       </c>
       <c r="F24" t="s">
         <v>40</v>
@@ -7430,8 +7524,8 @@
       <c r="AU24">
         <v>0</v>
       </c>
-      <c r="AV24" s="4">
-        <v>1</v>
+      <c r="AV24" s="7">
+        <v>0</v>
       </c>
       <c r="AW24">
         <v>0</v>
@@ -7440,6 +7534,12 @@
         <v>21</v>
       </c>
       <c r="AZ24">
+        <v>1.0956188175599648E-2</v>
+      </c>
+      <c r="BA24" s="7">
+        <v>1</v>
+      </c>
+      <c r="BB24">
         <v>1.0956188175599648E-2</v>
       </c>
       <c r="BD24" t="s">
@@ -7460,13 +7560,15 @@
         <v>41</v>
       </c>
       <c r="B25">
-        <v>7.7111503449062216E-3</v>
-      </c>
-      <c r="C25">
+        <f t="shared" ref="B25" ca="1" si="22">(#REF!/B$35)*100</f>
+        <v>7.7005467287947198E-3</v>
+      </c>
+      <c r="C25" s="5">
         <v>0.51803644477500932</v>
       </c>
-      <c r="D25">
-        <v>3.9946569098008059E-3</v>
+      <c r="D25" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.9891638502086444E-3</v>
       </c>
       <c r="F25" t="s">
         <v>31</v>
@@ -7570,17 +7672,23 @@
       <c r="AU25">
         <v>1.4113168701338675E-2</v>
       </c>
-      <c r="AV25" s="4">
-        <v>0</v>
+      <c r="AV25" s="7">
+        <v>1</v>
       </c>
       <c r="AW25">
-        <v>0</v>
+        <v>1.4113168701338675E-2</v>
       </c>
       <c r="AY25" t="s">
         <v>42</v>
       </c>
       <c r="AZ25">
         <v>8.0673262145865845</v>
+      </c>
+      <c r="BA25" s="7">
+        <v>0.36940295466953504</v>
+      </c>
+      <c r="BB25">
+        <v>2.9800941399512797</v>
       </c>
       <c r="BD25" t="s">
         <v>79</v>
@@ -7600,13 +7708,15 @@
         <v>42</v>
       </c>
       <c r="B26">
-        <v>31.301575218249724</v>
-      </c>
-      <c r="C26">
+        <f t="shared" ref="B26" ca="1" si="23">(#REF!/B$35)*100</f>
+        <v>31.258532368291696</v>
+      </c>
+      <c r="C26" s="5">
         <v>0.52182050165299265</v>
       </c>
-      <c r="D26">
-        <v>16.333803682915953</v>
+      <c r="D26" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>16.311343041358281</v>
       </c>
       <c r="F26" t="s">
         <v>42</v>
@@ -7710,17 +7820,23 @@
       <c r="AU26">
         <v>20.944528049287698</v>
       </c>
-      <c r="AV26" s="4">
-        <v>1</v>
+      <c r="AV26" s="7">
+        <v>0.62025893480741623</v>
       </c>
       <c r="AW26">
-        <v>20.944528049287698</v>
+        <v>12.991030657895239</v>
       </c>
       <c r="AY26" t="s">
         <v>30</v>
       </c>
       <c r="AZ26">
         <v>2.3062118738346724</v>
+      </c>
+      <c r="BA26" s="7">
+        <v>0.86077512898229869</v>
+      </c>
+      <c r="BB26">
+        <v>1.985129823160549</v>
       </c>
       <c r="BD26" t="s">
         <v>80</v>
@@ -7740,13 +7856,15 @@
         <v>43</v>
       </c>
       <c r="B27">
-        <v>0.51339227368831197</v>
-      </c>
-      <c r="C27">
+        <f t="shared" ref="B27" ca="1" si="24">(#REF!/B$35)*100</f>
+        <v>0.51268630708912644</v>
+      </c>
+      <c r="C27" s="5">
         <v>0.67819558951672365</v>
       </c>
-      <c r="D27">
-        <v>0.34818037570737587</v>
+      <c r="D27" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.34770159227346215</v>
       </c>
       <c r="F27" t="s">
         <v>49</v>
@@ -7850,17 +7968,23 @@
       <c r="AU27">
         <v>6.3470024547034321</v>
       </c>
-      <c r="AV27" s="4">
-        <v>0.67724858098644825</v>
+      <c r="AV27" s="7">
+        <v>0.57192665691249267</v>
       </c>
       <c r="AW27">
-        <v>4.298498405965403</v>
+        <v>3.6300198953339184</v>
       </c>
       <c r="AY27" t="s">
         <v>36</v>
       </c>
       <c r="AZ27">
         <v>29.61594068407371</v>
+      </c>
+      <c r="BA27" s="7">
+        <v>0.77906345046260372</v>
+      </c>
+      <c r="BB27">
+        <v>23.072696938030269</v>
       </c>
       <c r="BD27" t="s">
         <v>72</v>
@@ -7880,13 +8004,15 @@
         <v>44</v>
       </c>
       <c r="B28">
-        <v>3.6151444297169153</v>
-      </c>
-      <c r="C28">
+        <f t="shared" ref="B28" ca="1" si="25">(#REF!/B$35)*100</f>
+        <v>3.6101732383893239</v>
+      </c>
+      <c r="C28" s="5">
         <v>0.57076383920143292</v>
       </c>
-      <c r="D28">
-        <v>2.0633937139729013</v>
+      <c r="D28" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.0605563377253606</v>
       </c>
       <c r="F28" t="s">
         <v>28</v>
@@ -7990,16 +8116,22 @@
       <c r="AU28">
         <v>9.5031515411368535</v>
       </c>
-      <c r="AV28" s="4">
-        <v>0.56168699774527375</v>
+      <c r="AV28" s="7">
+        <v>0.75394944854374402</v>
       </c>
       <c r="AW28">
-        <v>5.3377966582595304</v>
+        <v>7.1648958638677618</v>
       </c>
       <c r="AY28" t="s">
         <v>61</v>
       </c>
       <c r="AZ28">
+        <v>0.89612854325864622</v>
+      </c>
+      <c r="BA28" s="7">
+        <v>1</v>
+      </c>
+      <c r="BB28">
         <v>0.89612854325864622</v>
       </c>
       <c r="BD28" t="s">
@@ -8020,13 +8152,15 @@
         <v>45</v>
       </c>
       <c r="B29">
-        <v>3.2184804471366011</v>
-      </c>
-      <c r="C29">
+        <f t="shared" ref="B29" ca="1" si="26">(#REF!/B$35)*100</f>
+        <v>3.2140547091341833</v>
+      </c>
+      <c r="C29" s="5">
         <v>0.4119287022145795</v>
       </c>
-      <c r="D29">
-        <v>1.3257844736919797</v>
+      <c r="D29" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.323961385180302</v>
       </c>
       <c r="F29" t="s">
         <v>20</v>
@@ -8130,17 +8264,23 @@
       <c r="AU29">
         <v>3.5192950302875654</v>
       </c>
-      <c r="AV29" s="4">
-        <v>0.45889491923632975</v>
+      <c r="AV29" s="7">
+        <v>1</v>
       </c>
       <c r="AW29">
-        <v>1.614986608692629</v>
+        <v>3.5192950302875654</v>
       </c>
       <c r="AY29" t="s">
         <v>59</v>
       </c>
       <c r="AZ29">
         <v>0.18658388463046202</v>
+      </c>
+      <c r="BA29" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="BB29">
+        <v>9.3291942315231011E-2</v>
       </c>
       <c r="BD29" t="s">
         <v>33</v>
@@ -8160,13 +8300,15 @@
         <v>46</v>
       </c>
       <c r="B30">
-        <v>2.0212605505506125</v>
-      </c>
-      <c r="C30">
+        <f t="shared" ref="B30" ca="1" si="27">(#REF!/B$35)*100</f>
+        <v>2.0184811116886121</v>
+      </c>
+      <c r="C30" s="5">
         <v>0.60908383468433869</v>
       </c>
-      <c r="D30">
-        <v>1.2311171270255448</v>
+      <c r="D30" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.2294242157452069</v>
       </c>
       <c r="F30" t="s">
         <v>21</v>
@@ -8261,16 +8403,22 @@
       <c r="AU30">
         <v>1.0881253068732119E-2</v>
       </c>
-      <c r="AV30" s="4">
-        <v>0.61902852273296904</v>
+      <c r="AV30" s="7">
+        <v>1</v>
       </c>
       <c r="AW30">
-        <v>6.7358060126208302E-3</v>
+        <v>1.0881253068732119E-2</v>
       </c>
       <c r="AY30" t="s">
         <v>58</v>
       </c>
       <c r="AZ30">
+        <v>2.8490143046184055</v>
+      </c>
+      <c r="BA30" s="7">
+        <v>1</v>
+      </c>
+      <c r="BB30">
         <v>2.8490143046184055</v>
       </c>
       <c r="BD30" t="s">
@@ -8291,13 +8439,15 @@
         <v>47</v>
       </c>
       <c r="B31">
-        <v>5.0248554119879953</v>
-      </c>
-      <c r="C31">
+        <f t="shared" ref="B31" ca="1" si="28">(#REF!/B$35)*100</f>
+        <v>5.0179457246623276</v>
+      </c>
+      <c r="C31" s="5">
         <v>0.4164950536354331</v>
       </c>
-      <c r="D31">
-        <v>2.0928274243262366</v>
+      <c r="D31" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.0899495737329286</v>
       </c>
       <c r="F31" t="s">
         <v>43</v>
@@ -8389,17 +8539,23 @@
       <c r="AU31">
         <v>0.25403703662409616</v>
       </c>
-      <c r="AV31" s="4">
-        <v>1</v>
+      <c r="AV31" s="7">
+        <v>0.77777777777777779</v>
       </c>
       <c r="AW31">
-        <v>0.25403703662409616</v>
+        <v>0.19758436181874145</v>
       </c>
       <c r="AY31" t="s">
         <v>28</v>
       </c>
       <c r="AZ31">
         <v>10.188679803428451</v>
+      </c>
+      <c r="BA31" s="7">
+        <v>0.49251382470515814</v>
+      </c>
+      <c r="BB31">
+        <v>5.0180656586827457</v>
       </c>
       <c r="BD31" t="s">
         <v>25</v>
@@ -8419,13 +8575,15 @@
         <v>48</v>
       </c>
       <c r="B32">
-        <v>0.6443527846407765</v>
-      </c>
-      <c r="C32">
+        <f t="shared" ref="B32" ca="1" si="29">(#REF!/B$35)*100</f>
+        <v>0.6434667340175747</v>
+      </c>
+      <c r="C32" s="5">
         <v>0.85671307010360664</v>
       </c>
-      <c r="D32">
-        <v>0.5520254523594077</v>
+      <c r="D32" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.55126636120973727</v>
       </c>
       <c r="F32" t="s">
         <v>45</v>
@@ -8517,11 +8675,11 @@
       <c r="AU32">
         <v>0.87879173211060613</v>
       </c>
-      <c r="AV32" s="4">
-        <v>1</v>
+      <c r="AV32" s="7">
+        <v>0.84400369374071538</v>
       </c>
       <c r="AW32">
-        <v>0.87879173211060613</v>
+        <v>0.74170346793015285</v>
       </c>
       <c r="AY32" t="s">
         <v>45</v>
@@ -8529,8 +8687,14 @@
       <c r="AZ32">
         <v>4.0491058545268004</v>
       </c>
+      <c r="BA32" s="7">
+        <v>0.57769449837312026</v>
+      </c>
+      <c r="BB32">
+        <v>2.3391461754905243</v>
+      </c>
       <c r="BD32" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="BE32">
         <v>0.60865679927950467</v>
@@ -8547,13 +8711,15 @@
         <v>49</v>
       </c>
       <c r="B33">
-        <v>21.885882115380461</v>
-      </c>
-      <c r="C33">
+        <f t="shared" ref="B33" ca="1" si="30">(#REF!/B$35)*100</f>
+        <v>21.855786801214222</v>
+      </c>
+      <c r="C33" s="5">
         <v>0.24939507620133408</v>
       </c>
-      <c r="D33">
-        <v>5.4582312378987252</v>
+      <c r="D33" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.4507256147289329</v>
       </c>
       <c r="I33">
         <v>70.445705838563896</v>
@@ -8630,11 +8796,11 @@
       <c r="AU33">
         <v>1.5789036918779138</v>
       </c>
-      <c r="AV33" s="4">
-        <v>0.84400369374071538</v>
+      <c r="AV33" s="7">
+        <v>0.35706081367961418</v>
       </c>
       <c r="AW33">
-        <v>1.3326005480058116</v>
+        <v>0.56376463694367474</v>
       </c>
       <c r="AY33" t="s">
         <v>46</v>
@@ -8642,8 +8808,14 @@
       <c r="AZ33">
         <v>0.41085705658498678</v>
       </c>
+      <c r="BA33" s="7">
+        <v>0.70666666666666667</v>
+      </c>
+      <c r="BB33">
+        <v>0.29033898665339064</v>
+      </c>
       <c r="BD33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="BE33">
         <v>0.52060137027106468</v>
@@ -8660,13 +8832,15 @@
         <v>50</v>
       </c>
       <c r="B34">
-        <v>5.6797583350143839</v>
-      </c>
-      <c r="C34">
+        <f t="shared" ref="B34" ca="1" si="31">(#REF!/B$35)*100</f>
+        <v>5.6719480895520622</v>
+      </c>
+      <c r="C34" s="5">
         <v>0.60192974780895803</v>
       </c>
-      <c r="D34">
-        <v>3.4188155022110354</v>
+      <c r="D34" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.4141142831295741</v>
       </c>
       <c r="N34">
         <v>77.656074018251672</v>
@@ -8716,14 +8890,23 @@
       <c r="AU34">
         <v>3.4835887134731793</v>
       </c>
+      <c r="AV34" s="7">
+        <v>0.78512959192974985</v>
+      </c>
       <c r="AW34">
-        <v>0</v>
+        <v>2.7350685850602794</v>
       </c>
       <c r="AY34" t="s">
         <v>69</v>
       </c>
       <c r="AZ34">
         <v>9.8605693580396836E-2</v>
+      </c>
+      <c r="BA34" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="BB34">
+        <v>3.2868564526798941E-2</v>
       </c>
       <c r="BD34" t="s">
         <v>39</v>
@@ -8743,13 +8926,15 @@
         <v>51</v>
       </c>
       <c r="B35">
-        <v>4.0379529112539085</v>
-      </c>
-      <c r="C35">
+        <f t="shared" ref="B35" ca="1" si="32">(#REF!/B$35)*100</f>
+        <v>4.0324003152556296</v>
+      </c>
+      <c r="C35" s="5">
         <v>0.31312025157339896</v>
       </c>
-      <c r="D35">
-        <v>1.2643648314133626</v>
+      <c r="D35" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.262626201157496</v>
       </c>
       <c r="U35" t="s">
         <v>40</v>
@@ -8793,11 +8978,17 @@
       <c r="AU35">
         <v>4.979125917832284E-2</v>
       </c>
+      <c r="AV35" s="7">
+        <v>1</v>
+      </c>
       <c r="AW35">
-        <v>0</v>
+        <v>4.979125917832284E-2</v>
+      </c>
+      <c r="BB35">
+        <v>62.382667441780463</v>
       </c>
       <c r="BD35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="BE35">
         <v>1.3277120869189138</v>
@@ -8810,8 +9001,9 @@
       </c>
     </row>
     <row r="36" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="D36">
-        <v>49.544697292971854</v>
+      <c r="D36" s="2">
+        <f ca="1">SUM(D3:D35)</f>
+        <v>49.646959715186867</v>
       </c>
       <c r="U36" t="s">
         <v>49</v>
@@ -8855,11 +9047,14 @@
       <c r="AU36">
         <v>4.995560702784994</v>
       </c>
+      <c r="AV36" s="7">
+        <v>0.99106548820573825</v>
+      </c>
       <c r="AW36">
-        <v>0</v>
+        <v>4.9509278067670106</v>
       </c>
       <c r="BD36" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="BE36">
         <v>0.33447860879470359</v>
@@ -8900,10 +9095,10 @@
         <v>1.8427235022645573E-3</v>
       </c>
       <c r="AW37">
-        <v>59.496626987580697</v>
+        <v>71.950218337776391</v>
       </c>
       <c r="BD37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="BE37">
         <v>1.3188011834034088</v>
@@ -8941,7 +9136,7 @@
         <v>1.021737746784088E-2</v>
       </c>
       <c r="BD38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="BE38">
         <v>1.9407687553222586E-2</v>
@@ -8979,7 +9174,7 @@
         <v>9.8316040517163871E-3</v>
       </c>
       <c r="BD39" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="BE39">
         <v>5.193606528327171E-3</v>
@@ -9017,7 +9212,7 @@
         <v>0.1086172207052551</v>
       </c>
       <c r="BD40" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="BE40">
         <v>1.2194844373875319E-3</v>
@@ -9046,7 +9241,7 @@
         <v>4.7902383969691306E-2</v>
       </c>
       <c r="BD41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="BE41">
         <v>1.4225797583240845</v>
@@ -9072,7 +9267,7 @@
         <v>0.11439867205928585</v>
       </c>
       <c r="BD42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="BE42">
         <v>1.11707006466164</v>
@@ -9187,7 +9382,7 @@
     </row>
     <row r="50" spans="56:59" x14ac:dyDescent="0.25">
       <c r="BD50" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="BE50">
         <v>1.4565983593706556E-2</v>
@@ -9215,7 +9410,7 @@
     </row>
     <row r="52" spans="56:59" x14ac:dyDescent="0.25">
       <c r="BD52" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="BE52">
         <v>0.62147385029584556</v>
@@ -9313,7 +9508,7 @@
     </row>
     <row r="59" spans="56:59" x14ac:dyDescent="0.25">
       <c r="BD59" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="BE59">
         <v>0.11686063987732562</v>
@@ -9327,7 +9522,7 @@
     </row>
     <row r="60" spans="56:59" x14ac:dyDescent="0.25">
       <c r="BD60" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="BE60">
         <v>7.6491782329689189</v>
@@ -9341,7 +9536,7 @@
     </row>
     <row r="61" spans="56:59" x14ac:dyDescent="0.25">
       <c r="BD61" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="BE61">
         <v>3.6723165051648015</v>
@@ -9355,7 +9550,7 @@
     </row>
     <row r="62" spans="56:59" x14ac:dyDescent="0.25">
       <c r="BD62" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="BE62">
         <v>2.9155664810771218</v>
@@ -9369,7 +9564,7 @@
     </row>
     <row r="63" spans="56:59" x14ac:dyDescent="0.25">
       <c r="BD63" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="BE63">
         <v>0.1706502809235815</v>
@@ -9510,6 +9705,205 @@
     <row r="73" spans="56:59" x14ac:dyDescent="0.25">
       <c r="BG73">
         <v>49.148754824102483</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BG2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" t="s">
+        <v>17</v>
+      </c>
+      <c r="X2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>17</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>15</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>17</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>